<commit_message>
Use pricer-based ownership for costs; keep owner for reporting
</commit_message>
<xml_diff>
--- a/post_est/data/raw/brand_owner_hq.xlsx
+++ b/post_est/data/raw/brand_owner_hq.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukeheeney/Documents/CEEPR/EV_IO/code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukeheeney/Documents/CEEPR/EV_IO/code/replication_repo/post_est/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1182A8F9-A51C-F34E-950D-33458E277BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5138C9-3867-3649-8064-D0DBFB5680CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="107">
   <si>
     <t>brand</t>
   </si>
@@ -35,24 +35,15 @@
     <t>honda</t>
   </si>
   <si>
-    <t>japan</t>
-  </si>
-  <si>
     <t>astonmartin</t>
   </si>
   <si>
-    <t>united kingdom</t>
-  </si>
-  <si>
     <t>audi</t>
   </si>
   <si>
     <t>volkswagen</t>
   </si>
   <si>
-    <t>germany</t>
-  </si>
-  <si>
     <t>bentley</t>
   </si>
   <si>
@@ -65,9 +56,6 @@
     <t>generalmotors</t>
   </si>
   <si>
-    <t>united states</t>
-  </si>
-  <si>
     <t>cadillac</t>
   </si>
   <si>
@@ -80,18 +68,12 @@
     <t>stellantis</t>
   </si>
   <si>
-    <t>netherlands</t>
-  </si>
-  <si>
     <t>dodge</t>
   </si>
   <si>
     <t>ferrari</t>
   </si>
   <si>
-    <t>italy</t>
-  </si>
-  <si>
     <t>fiat</t>
   </si>
   <si>
@@ -104,9 +86,6 @@
     <t>hyundai</t>
   </si>
   <si>
-    <t>south korea</t>
-  </si>
-  <si>
     <t>infiniti</t>
   </si>
   <si>
@@ -119,9 +98,6 @@
     <t>tatamotors</t>
   </si>
   <si>
-    <t>india</t>
-  </si>
-  <si>
     <t>jeep</t>
   </si>
   <si>
@@ -149,9 +125,6 @@
     <t>geely</t>
   </si>
   <si>
-    <t>china</t>
-  </si>
-  <si>
     <t>maserati</t>
   </si>
   <si>
@@ -200,9 +173,6 @@
     <t>polestar</t>
   </si>
   <si>
-    <t>sweden</t>
-  </si>
-  <si>
     <t>lucidmotors</t>
   </si>
   <si>
@@ -365,7 +335,13 @@
     <t>https://en.wikipedia.org/wiki/Rivian</t>
   </si>
   <si>
-    <t>hqcountry (owner)</t>
+    <t>pricer</t>
+  </si>
+  <si>
+    <t>stellantis_a</t>
+  </si>
+  <si>
+    <t>stellantis_b</t>
   </si>
 </sst>
 </file>
@@ -441,13 +417,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BrandOwners" displayName="BrandOwners" ref="A1:C46">
   <autoFilter ref="A1:C46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C46">
-    <sortCondition ref="B1:B46"/>
-  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="brand"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="owner"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="hqcountry (owner)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="pricer"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -632,7 +605,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -650,161 +623,161 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -815,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -826,326 +799,326 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1173,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1184,153 +1157,153 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -1338,340 +1311,340 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>